<commit_message>
lsmm & lvst update
</commit_message>
<xml_diff>
--- a/ssp_modeling/scenario_mapping/ssp_uganda_transformation_cw_asp.xlsx
+++ b/ssp_modeling/scenario_mapping/ssp_uganda_transformation_cw_asp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\fabian_fuentes\repos\ssp_uganda_private\ssp_modeling\scenario_mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33420DD0-AB03-4F02-8B6E-886AC36EAB29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0F79B6-D143-4202-B364-BE9656B57A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -2200,31 +2200,31 @@
   <dimension ref="A1:Q62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="K27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="M25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O33" sqref="O33"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.21875" style="19" customWidth="1"/>
-    <col min="3" max="3" width="43.44140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.44140625" style="19" customWidth="1"/>
-    <col min="5" max="5" width="62.5546875" style="19" customWidth="1"/>
-    <col min="6" max="6" width="33.21875" style="19" customWidth="1"/>
-    <col min="7" max="7" width="19.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="47.44140625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="48.5546875" style="16" customWidth="1"/>
-    <col min="10" max="10" width="40.44140625" style="16" customWidth="1"/>
+    <col min="1" max="2" width="13.28515625" style="19" customWidth="1"/>
+    <col min="3" max="3" width="43.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.42578125" style="19" customWidth="1"/>
+    <col min="5" max="5" width="62.5703125" style="19" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" style="19" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="47.42578125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="48.5703125" style="16" customWidth="1"/>
+    <col min="10" max="10" width="40.42578125" style="16" customWidth="1"/>
     <col min="11" max="12" width="35" style="16" customWidth="1"/>
-    <col min="13" max="13" width="31.44140625" style="41" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="4" customWidth="1"/>
-    <col min="15" max="17" width="20.44140625" style="29" customWidth="1"/>
-    <col min="18" max="16384" width="8.77734375" style="15"/>
+    <col min="13" max="13" width="31.42578125" style="41" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" style="4" customWidth="1"/>
+    <col min="15" max="17" width="20.42578125" style="29" customWidth="1"/>
+    <col min="18" max="16384" width="8.7109375" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="5" customFormat="1" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="5" customFormat="1" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="12" customFormat="1" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" s="12" customFormat="1" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -2324,7 +2324,7 @@
       </c>
       <c r="Q2" s="11"/>
     </row>
-    <row r="3" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
@@ -2363,7 +2363,7 @@
       </c>
       <c r="Q3" s="11"/>
     </row>
-    <row r="4" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
@@ -2402,7 +2402,7 @@
       </c>
       <c r="Q4" s="11"/>
     </row>
-    <row r="5" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
@@ -2446,7 +2446,7 @@
       </c>
       <c r="Q5" s="11"/>
     </row>
-    <row r="6" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>80</v>
       </c>
@@ -2538,7 +2538,7 @@
       </c>
       <c r="Q7" s="42"/>
     </row>
-    <row r="8" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>80</v>
       </c>
@@ -2589,7 +2589,7 @@
       </c>
       <c r="Q8" s="11"/>
     </row>
-    <row r="9" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>80</v>
       </c>
@@ -2640,7 +2640,7 @@
       </c>
       <c r="Q9" s="11"/>
     </row>
-    <row r="10" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>80</v>
       </c>
@@ -2691,7 +2691,7 @@
       </c>
       <c r="Q10" s="11"/>
     </row>
-    <row r="11" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>80</v>
       </c>
@@ -2730,7 +2730,7 @@
       </c>
       <c r="Q11" s="11"/>
     </row>
-    <row r="12" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>80</v>
       </c>
@@ -2769,7 +2769,7 @@
       </c>
       <c r="Q12" s="11"/>
     </row>
-    <row r="13" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>80</v>
       </c>
@@ -2820,7 +2820,7 @@
       </c>
       <c r="Q13" s="11"/>
     </row>
-    <row r="14" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>80</v>
       </c>
@@ -2871,7 +2871,7 @@
       </c>
       <c r="Q14" s="11"/>
     </row>
-    <row r="15" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>80</v>
       </c>
@@ -2910,7 +2910,7 @@
       </c>
       <c r="Q15" s="11"/>
     </row>
-    <row r="16" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>127</v>
       </c>
@@ -2961,7 +2961,7 @@
       </c>
       <c r="Q16" s="11"/>
     </row>
-    <row r="17" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>127</v>
       </c>
@@ -3012,7 +3012,7 @@
       </c>
       <c r="Q17" s="11"/>
     </row>
-    <row r="18" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>127</v>
       </c>
@@ -3063,7 +3063,7 @@
       </c>
       <c r="Q18" s="11"/>
     </row>
-    <row r="19" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>127</v>
       </c>
@@ -3102,7 +3102,7 @@
       </c>
       <c r="Q19" s="11"/>
     </row>
-    <row r="20" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>127</v>
       </c>
@@ -3141,7 +3141,7 @@
       </c>
       <c r="Q20" s="11"/>
     </row>
-    <row r="21" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>127</v>
       </c>
@@ -3180,7 +3180,7 @@
       </c>
       <c r="Q21" s="11"/>
     </row>
-    <row r="22" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>5</v>
       </c>
@@ -3231,7 +3231,7 @@
       </c>
       <c r="Q22" s="11"/>
     </row>
-    <row r="23" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>5</v>
       </c>
@@ -3276,7 +3276,7 @@
       <c r="P23" s="11"/>
       <c r="Q23" s="11"/>
     </row>
-    <row r="24" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>5</v>
       </c>
@@ -3327,7 +3327,7 @@
       </c>
       <c r="Q24" s="11"/>
     </row>
-    <row r="25" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>5</v>
       </c>
@@ -3372,7 +3372,7 @@
       <c r="P25" s="11"/>
       <c r="Q25" s="11"/>
     </row>
-    <row r="26" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>5</v>
       </c>
@@ -3410,14 +3410,14 @@
         <v>1</v>
       </c>
       <c r="O26" s="11">
-        <v>1</v>
+        <v>1.05</v>
       </c>
       <c r="P26" s="11">
-        <v>1</v>
+        <v>1.05</v>
       </c>
       <c r="Q26" s="11"/>
     </row>
-    <row r="27" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>5</v>
       </c>
@@ -3462,7 +3462,7 @@
       </c>
       <c r="Q27" s="11"/>
     </row>
-    <row r="28" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>5</v>
       </c>
@@ -3507,7 +3507,7 @@
       </c>
       <c r="Q28" s="11"/>
     </row>
-    <row r="29" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>5</v>
       </c>
@@ -3552,7 +3552,7 @@
       </c>
       <c r="Q29" s="11"/>
     </row>
-    <row r="30" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>5</v>
       </c>
@@ -3591,7 +3591,7 @@
       </c>
       <c r="Q30" s="11"/>
     </row>
-    <row r="31" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>5</v>
       </c>
@@ -3630,7 +3630,7 @@
       </c>
       <c r="Q31" s="11"/>
     </row>
-    <row r="32" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>5</v>
       </c>
@@ -3674,16 +3674,16 @@
         <v>248</v>
       </c>
       <c r="O32" s="11">
-        <v>2.5</v>
+        <v>1.2</v>
       </c>
       <c r="P32" s="11">
-        <v>2.5</v>
+        <v>1.2</v>
       </c>
       <c r="Q32" s="11">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>151</v>
       </c>
@@ -3720,7 +3720,7 @@
       <c r="P33" s="11"/>
       <c r="Q33" s="11"/>
     </row>
-    <row r="34" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>151</v>
       </c>
@@ -3759,7 +3759,7 @@
       </c>
       <c r="Q34" s="11"/>
     </row>
-    <row r="35" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>80</v>
       </c>
@@ -3798,7 +3798,7 @@
       </c>
       <c r="Q35" s="11"/>
     </row>
-    <row r="36" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>80</v>
       </c>
@@ -3837,7 +3837,7 @@
       </c>
       <c r="Q36" s="11"/>
     </row>
-    <row r="37" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>80</v>
       </c>
@@ -3876,7 +3876,7 @@
       </c>
       <c r="Q37" s="11"/>
     </row>
-    <row r="38" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>5</v>
       </c>
@@ -3917,7 +3917,7 @@
       </c>
       <c r="Q38" s="11"/>
     </row>
-    <row r="39" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>5</v>
       </c>
@@ -3958,7 +3958,7 @@
       </c>
       <c r="Q39" s="11"/>
     </row>
-    <row r="40" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>80</v>
       </c>
@@ -4009,7 +4009,7 @@
       </c>
       <c r="Q40" s="11"/>
     </row>
-    <row r="41" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>80</v>
       </c>
@@ -4060,7 +4060,7 @@
       </c>
       <c r="Q41" s="11"/>
     </row>
-    <row r="42" spans="1:17" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>80</v>
       </c>
@@ -4111,7 +4111,7 @@
       </c>
       <c r="Q42" s="11"/>
     </row>
-    <row r="43" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>80</v>
       </c>
@@ -4150,7 +4150,7 @@
       </c>
       <c r="Q43" s="11"/>
     </row>
-    <row r="44" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>80</v>
       </c>
@@ -4189,7 +4189,7 @@
       </c>
       <c r="Q44" s="11"/>
     </row>
-    <row r="45" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>80</v>
       </c>
@@ -4240,7 +4240,7 @@
       </c>
       <c r="Q45" s="11"/>
     </row>
-    <row r="46" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>80</v>
       </c>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="Q46" s="11"/>
     </row>
-    <row r="47" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>80</v>
       </c>
@@ -4330,7 +4330,7 @@
       </c>
       <c r="Q47" s="11"/>
     </row>
-    <row r="48" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>80</v>
       </c>
@@ -4381,7 +4381,7 @@
       </c>
       <c r="Q48" s="11"/>
     </row>
-    <row r="49" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>80</v>
       </c>
@@ -4432,7 +4432,7 @@
       </c>
       <c r="Q49" s="11"/>
     </row>
-    <row r="50" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>80</v>
       </c>
@@ -4483,7 +4483,7 @@
       </c>
       <c r="Q50" s="11"/>
     </row>
-    <row r="51" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>127</v>
       </c>
@@ -4522,7 +4522,7 @@
       </c>
       <c r="Q51" s="11"/>
     </row>
-    <row r="52" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>127</v>
       </c>
@@ -4573,7 +4573,7 @@
       </c>
       <c r="Q52" s="11"/>
     </row>
-    <row r="53" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>57</v>
       </c>
@@ -4624,7 +4624,7 @@
       </c>
       <c r="Q53" s="11"/>
     </row>
-    <row r="54" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>57</v>
       </c>
@@ -4675,7 +4675,7 @@
       </c>
       <c r="Q54" s="11"/>
     </row>
-    <row r="55" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>57</v>
       </c>
@@ -4726,7 +4726,7 @@
       </c>
       <c r="Q55" s="11"/>
     </row>
-    <row r="56" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>57</v>
       </c>
@@ -4777,7 +4777,7 @@
       </c>
       <c r="Q56" s="11"/>
     </row>
-    <row r="57" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>57</v>
       </c>
@@ -4820,7 +4820,7 @@
       </c>
       <c r="Q57" s="11"/>
     </row>
-    <row r="58" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>57</v>
       </c>
@@ -4869,7 +4869,7 @@
       </c>
       <c r="Q58" s="11"/>
     </row>
-    <row r="59" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>57</v>
       </c>
@@ -4914,7 +4914,7 @@
       </c>
       <c r="Q59" s="11"/>
     </row>
-    <row r="60" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>57</v>
       </c>
@@ -4959,7 +4959,7 @@
       </c>
       <c r="Q60" s="11"/>
     </row>
-    <row r="61" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>57</v>
       </c>
@@ -5010,7 +5010,7 @@
       </c>
       <c r="Q61" s="11"/>
     </row>
-    <row r="62" spans="1:17" ht="85.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>57</v>
       </c>
@@ -5630,17 +5630,17 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="19.21875" customWidth="1"/>
-    <col min="10" max="10" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="19.28515625" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>144</v>
       </c>
@@ -5669,7 +5669,7 @@
       <c r="I1" s="32"/>
       <c r="J1" s="32"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>145</v>
       </c>
@@ -5698,7 +5698,7 @@
       <c r="I2" s="35"/>
       <c r="J2" s="35"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>145</v>
       </c>
@@ -5727,7 +5727,7 @@
       <c r="I3" s="35"/>
       <c r="J3" s="35"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>145</v>
       </c>
@@ -5756,7 +5756,7 @@
       <c r="I4" s="35"/>
       <c r="J4" s="35"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>145</v>
       </c>
@@ -5785,7 +5785,7 @@
       <c r="I5" s="35"/>
       <c r="J5" s="35"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
         <v>145</v>
       </c>
@@ -5814,7 +5814,7 @@
       <c r="I6" s="35"/>
       <c r="J6" s="35"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>154</v>
       </c>
@@ -5843,7 +5843,7 @@
       <c r="I7" s="35"/>
       <c r="J7" s="35"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>155</v>
       </c>
@@ -5872,7 +5872,7 @@
       <c r="I8" s="35"/>
       <c r="J8" s="35"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
         <v>155</v>
       </c>
@@ -5901,7 +5901,7 @@
       <c r="I9" s="35"/>
       <c r="J9" s="35"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
         <v>155</v>
       </c>
@@ -5930,7 +5930,7 @@
       <c r="I10" s="35"/>
       <c r="J10" s="35"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
         <v>156</v>
       </c>
@@ -5959,7 +5959,7 @@
       <c r="I11" s="35"/>
       <c r="J11" s="35"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
         <v>156</v>
       </c>
@@ -5988,7 +5988,7 @@
       <c r="I12" s="35"/>
       <c r="J12" s="35"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
         <v>157</v>
       </c>
@@ -6017,7 +6017,7 @@
       <c r="I13" s="35"/>
       <c r="J13" s="35"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
         <v>157</v>
       </c>
@@ -6046,7 +6046,7 @@
       <c r="I14" s="35"/>
       <c r="J14" s="35"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
         <v>157</v>
       </c>
@@ -6075,7 +6075,7 @@
       <c r="I15" s="35"/>
       <c r="J15" s="35"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
         <v>127</v>
       </c>
@@ -6104,7 +6104,7 @@
       <c r="I16" s="35"/>
       <c r="J16" s="35"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
         <v>127</v>
       </c>
@@ -6133,7 +6133,7 @@
       <c r="I17" s="35"/>
       <c r="J17" s="35"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
         <v>127</v>
       </c>
@@ -6162,7 +6162,7 @@
       <c r="I18" s="35"/>
       <c r="J18" s="35"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="33" t="s">
         <v>127</v>
       </c>
@@ -6191,7 +6191,7 @@
       <c r="I19" s="35"/>
       <c r="J19" s="35"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="33" t="s">
         <v>127</v>
       </c>
@@ -6220,7 +6220,7 @@
       <c r="I20" s="35"/>
       <c r="J20" s="35"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="33" t="s">
         <v>127</v>
       </c>
@@ -6249,7 +6249,7 @@
       <c r="I21" s="35"/>
       <c r="J21" s="35"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="33" t="s">
         <v>146</v>
       </c>
@@ -6278,7 +6278,7 @@
       <c r="I22" s="35"/>
       <c r="J22" s="35"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
         <v>146</v>
       </c>
@@ -6307,7 +6307,7 @@
       <c r="I23" s="35"/>
       <c r="J23" s="35"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="33" t="s">
         <v>146</v>
       </c>
@@ -6336,7 +6336,7 @@
       <c r="I24" s="35"/>
       <c r="J24" s="35"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="33" t="s">
         <v>146</v>
       </c>
@@ -6365,7 +6365,7 @@
       <c r="I25" s="35"/>
       <c r="J25" s="35"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
         <v>147</v>
       </c>
@@ -6380,11 +6380,11 @@
       </c>
       <c r="E26" s="35">
         <f>+IF(VLOOKUP(B26,main!$C$2:$P$62,13,FALSE)=0,"",VLOOKUP(B26,main!$C$2:$P$62,13,FALSE))</f>
-        <v>1</v>
+        <v>1.05</v>
       </c>
       <c r="F26" s="35">
         <f>+IF(VLOOKUP(B26,main!C26:P86,14,FALSE)=0,"",VLOOKUP(B26,main!C26:P86,14,FALSE))</f>
-        <v>1</v>
+        <v>1.05</v>
       </c>
       <c r="G26" s="35" t="str">
         <f>+IF(VLOOKUP(B26,main!C26:Q86,15,FALSE)=0,"",VLOOKUP(B26,main!C26:Q86,15,FALSE))</f>
@@ -6394,7 +6394,7 @@
       <c r="I26" s="35"/>
       <c r="J26" s="35"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
         <v>147</v>
       </c>
@@ -6423,7 +6423,7 @@
       <c r="I27" s="35"/>
       <c r="J27" s="35"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
         <v>147</v>
       </c>
@@ -6452,7 +6452,7 @@
       <c r="I28" s="35"/>
       <c r="J28" s="35"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
         <v>147</v>
       </c>
@@ -6481,7 +6481,7 @@
       <c r="I29" s="35"/>
       <c r="J29" s="35"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="33" t="s">
         <v>148</v>
       </c>
@@ -6510,7 +6510,7 @@
       <c r="I30" s="35"/>
       <c r="J30" s="35"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="33" t="s">
         <v>148</v>
       </c>
@@ -6539,7 +6539,7 @@
       <c r="I31" s="35"/>
       <c r="J31" s="35"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="33" t="s">
         <v>148</v>
       </c>
@@ -6554,21 +6554,21 @@
       </c>
       <c r="E32" s="35">
         <f>+IF(VLOOKUP(B32,main!$C$2:$P$62,13,FALSE)=0,"",VLOOKUP(B32,main!$C$2:$P$62,13,FALSE))</f>
-        <v>2.5</v>
+        <v>1.2</v>
       </c>
       <c r="F32" s="35">
         <f>+IF(VLOOKUP(B32,main!C32:P92,14,FALSE)=0,"",VLOOKUP(B32,main!C32:P92,14,FALSE))</f>
-        <v>2.5</v>
+        <v>1.2</v>
       </c>
       <c r="G32" s="35">
         <f>+IF(VLOOKUP(B32,main!C32:Q92,15,FALSE)=0,"",VLOOKUP(B32,main!C32:Q92,15,FALSE))</f>
-        <v>2.5</v>
+        <v>1.2</v>
       </c>
       <c r="H32" s="35"/>
       <c r="I32" s="35"/>
       <c r="J32" s="35"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="33" t="s">
         <v>150</v>
       </c>
@@ -6597,7 +6597,7 @@
       <c r="I33" s="35"/>
       <c r="J33" s="35"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="33" t="s">
         <v>150</v>
       </c>
@@ -6626,7 +6626,7 @@
       <c r="I34" s="35"/>
       <c r="J34" s="35"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="33" t="s">
         <v>158</v>
       </c>
@@ -6655,7 +6655,7 @@
       <c r="I35" s="35"/>
       <c r="J35" s="35"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="33" t="s">
         <v>158</v>
       </c>
@@ -6684,7 +6684,7 @@
       <c r="I36" s="35"/>
       <c r="J36" s="35"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="33" t="s">
         <v>158</v>
       </c>
@@ -6713,7 +6713,7 @@
       <c r="I37" s="35"/>
       <c r="J37" s="35"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="33" t="s">
         <v>149</v>
       </c>
@@ -6742,7 +6742,7 @@
       <c r="I38" s="35"/>
       <c r="J38" s="35"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="33" t="s">
         <v>149</v>
       </c>
@@ -6771,7 +6771,7 @@
       <c r="I39" s="35"/>
       <c r="J39" s="35"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="33" t="s">
         <v>159</v>
       </c>
@@ -6800,7 +6800,7 @@
       <c r="I40" s="35"/>
       <c r="J40" s="35"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="33" t="s">
         <v>160</v>
       </c>
@@ -6829,7 +6829,7 @@
       <c r="I41" s="35"/>
       <c r="J41" s="35"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="33" t="s">
         <v>160</v>
       </c>
@@ -6858,7 +6858,7 @@
       <c r="I42" s="35"/>
       <c r="J42" s="35"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="33" t="s">
         <v>160</v>
       </c>
@@ -6887,7 +6887,7 @@
       <c r="I43" s="35"/>
       <c r="J43" s="35"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="33" t="s">
         <v>160</v>
       </c>
@@ -6916,7 +6916,7 @@
       <c r="I44" s="35"/>
       <c r="J44" s="35"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="33" t="s">
         <v>160</v>
       </c>
@@ -6945,7 +6945,7 @@
       <c r="I45" s="35"/>
       <c r="J45" s="35"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="33" t="s">
         <v>160</v>
       </c>
@@ -6974,7 +6974,7 @@
       <c r="I46" s="35"/>
       <c r="J46" s="35"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="33" t="s">
         <v>160</v>
       </c>
@@ -7003,7 +7003,7 @@
       <c r="I47" s="35"/>
       <c r="J47" s="35"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="33" t="s">
         <v>160</v>
       </c>
@@ -7032,7 +7032,7 @@
       <c r="I48" s="35"/>
       <c r="J48" s="35"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="33" t="s">
         <v>160</v>
       </c>
@@ -7061,7 +7061,7 @@
       <c r="I49" s="35"/>
       <c r="J49" s="35"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="33" t="s">
         <v>160</v>
       </c>
@@ -7090,7 +7090,7 @@
       <c r="I50" s="35"/>
       <c r="J50" s="35"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="33" t="s">
         <v>161</v>
       </c>
@@ -7119,7 +7119,7 @@
       <c r="I51" s="35"/>
       <c r="J51" s="35"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="33" t="s">
         <v>161</v>
       </c>
@@ -7148,7 +7148,7 @@
       <c r="I52" s="35"/>
       <c r="J52" s="35"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="33" t="s">
         <v>152</v>
       </c>
@@ -7177,7 +7177,7 @@
       <c r="I53" s="35"/>
       <c r="J53" s="35"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="33" t="s">
         <v>152</v>
       </c>
@@ -7206,7 +7206,7 @@
       <c r="I54" s="35"/>
       <c r="J54" s="35"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="33" t="s">
         <v>152</v>
       </c>
@@ -7235,7 +7235,7 @@
       <c r="I55" s="35"/>
       <c r="J55" s="35"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="33" t="s">
         <v>153</v>
       </c>
@@ -7264,7 +7264,7 @@
       <c r="I56" s="35"/>
       <c r="J56" s="35"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="33" t="s">
         <v>153</v>
       </c>
@@ -7293,7 +7293,7 @@
       <c r="I57" s="35"/>
       <c r="J57" s="35"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="33" t="s">
         <v>153</v>
       </c>
@@ -7322,7 +7322,7 @@
       <c r="I58" s="35"/>
       <c r="J58" s="35"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="33" t="s">
         <v>153</v>
       </c>
@@ -7351,7 +7351,7 @@
       <c r="I59" s="35"/>
       <c r="J59" s="35"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="33" t="s">
         <v>153</v>
       </c>
@@ -7380,7 +7380,7 @@
       <c r="I60" s="35"/>
       <c r="J60" s="35"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="33" t="s">
         <v>153</v>
       </c>
@@ -7409,7 +7409,7 @@
       <c r="I61" s="35"/>
       <c r="J61" s="35"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="33" t="s">
         <v>153</v>
       </c>

</xml_diff>